<commit_message>
Deploying to gh-pages from  @ adcabfb090e71dd97f455647f67a09f9ddd7f34d 🚀
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20351"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dauerausleihe04\Documents\SDG\SdgTestEnvironment\sdg-indicators\public\AddInfos\de\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\G2\Nachhaltigkeit\international\b_Daten\Indikatoren\SDG 7\7-1-2\Daten\ZusätzlicheInformationenDe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD1F4DE-1618-49EC-8A6B-D1F60E4AD9AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="28512" windowHeight="13296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>Jahr</t>
   </si>
@@ -45,9 +44,6 @@
     <t>Weltgesundheitsorganisation (WHO)</t>
   </si>
   <si>
-    <t>©       Statistisches Bundesamt (Destatis) 2021</t>
-  </si>
-  <si>
     <t>Anteil der Bevölkerung, der vorwiegend saubere Energieträger und Technologien nutzt</t>
   </si>
   <si>
@@ -59,11 +55,14 @@
   <si>
     <t>Alle Daten geschätzt.</t>
   </si>
+  <si>
+    <t>©       Statistisches Bundesamt (Destatis) 2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,6 +223,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -240,10 +240,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$11</c:f>
+              <c:f>Tabelle2!$A$1:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -276,16 +276,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$1:$B$11</c:f>
+              <c:f>Tabelle2!$B$1:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>95</c:v>
                 </c:pt>
@@ -317,6 +320,9 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
@@ -338,10 +344,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$11</c:f>
+              <c:f>Tabelle2!$A$1:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -374,16 +380,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$C$1:$C$11</c:f>
+              <c:f>Tabelle2!$C$1:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -415,6 +424,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -482,6 +494,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -511,13 +524,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>283028</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -597,13 +610,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>149088</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>291945</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -722,23 +735,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -774,23 +770,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -966,22 +945,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -990,7 +969,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -999,12 +978,12 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1012,12 +991,12 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1025,7 +1004,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
@@ -1038,7 +1017,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2011</v>
       </c>
@@ -1051,7 +1030,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2012</v>
       </c>
@@ -1064,7 +1043,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -1077,7 +1056,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2014</v>
       </c>
@@ -1090,7 +1069,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2015</v>
       </c>
@@ -1103,7 +1082,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2016</v>
       </c>
@@ -1116,7 +1095,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2017</v>
       </c>
@@ -1129,7 +1108,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2018</v>
       </c>
@@ -1142,7 +1121,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2019</v>
       </c>
@@ -1155,7 +1134,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2020</v>
       </c>
@@ -1168,16 +1147,20 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1186,7 +1169,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1195,7 +1178,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1204,7 +1187,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1213,7 +1196,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1222,7 +1205,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1231,7 +1214,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1240,7 +1223,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1249,7 +1232,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1258,7 +1241,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1267,7 +1250,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1276,7 +1259,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1285,7 +1268,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1294,7 +1277,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1303,7 +1286,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1312,7 +1295,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1321,7 +1304,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1330,7 +1313,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1339,7 +1322,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1348,25 +1331,21 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="7"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
@@ -1374,12 +1353,12 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="1"/>
@@ -1387,10 +1366,12 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7" t="s">
-        <v>5</v>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="1"/>
@@ -1398,16 +1379,18 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1415,6 +1398,15 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1427,16 +1419,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>2010</v>
       </c>
@@ -1447,7 +1439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2011</v>
       </c>
@@ -1458,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2012</v>
       </c>
@@ -1469,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2013</v>
       </c>
@@ -1480,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2014</v>
       </c>
@@ -1491,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
@@ -1502,7 +1494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2016</v>
       </c>
@@ -1513,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2017</v>
       </c>
@@ -1524,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2018</v>
       </c>
@@ -1535,7 +1527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2019</v>
       </c>
@@ -1546,7 +1538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2020</v>
       </c>
@@ -1554,6 +1546,17 @@
         <v>95</v>
       </c>
       <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B12">
+        <v>95</v>
+      </c>
+      <c r="C12">
         <v>5</v>
       </c>
     </row>
@@ -1563,12 +1566,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>